<commit_message>
read as dataset product conversion dynamic
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABEACE02EC9F8B9A6E4E5BDE58AA" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{05528EDA-1699-495F-897D-3044AB3C4F39}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABEACE02EC9F8B9A6E4E5BDE58AA" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AAEF9F47-F111-4272-8140-18E79CEAF15B}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -822,11 +822,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AQ19" sqref="AQ19"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="7" max="7" width="26.83984375" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="14" max="14" width="7.89453125" customWidth="1"/>
+    <col min="15" max="15" width="11.7890625" customWidth="1"/>
+    <col min="28" max="28" width="14.83984375" customWidth="1"/>
+    <col min="29" max="29" width="13.68359375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
deleted obj bin from online repository
</commit_message>
<xml_diff>
--- a/product.xlsx
+++ b/product.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABEACE02EC9F8B9A6E4E5BDE58AA" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{AAEF9F47-F111-4272-8140-18E79CEAF15B}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABEACE02EC9F8B9A6E4E5BDE58AA" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{20FAB9EF-CECD-4C71-AEE5-1E6B1EFF15C5}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="161">
   <si>
     <t>Type</t>
   </si>
@@ -823,6 +824,1762 @@
   <dimension ref="A1:AU29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="7" max="7" width="26.83984375" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="14" max="14" width="7.89453125" customWidth="1"/>
+    <col min="15" max="15" width="11.7890625" customWidth="1"/>
+    <col min="28" max="28" width="14.83984375" customWidth="1"/>
+    <col min="29" max="29" width="13.68359375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>2</v>
+      </c>
+      <c r="W2">
+        <v>3</v>
+      </c>
+      <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
+        <v>90</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB3">
+        <v>-1</v>
+      </c>
+      <c r="AC3">
+        <v>-1</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>9</v>
+      </c>
+      <c r="X5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>9</v>
+      </c>
+      <c r="X6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+      <c r="W7">
+        <v>9</v>
+      </c>
+      <c r="X7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <v>9</v>
+      </c>
+      <c r="X8" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+      <c r="W9">
+        <v>15</v>
+      </c>
+      <c r="X9" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="W10">
+        <v>15</v>
+      </c>
+      <c r="X10" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>12</v>
+      </c>
+      <c r="W11">
+        <v>15</v>
+      </c>
+      <c r="X11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>12</v>
+      </c>
+      <c r="W12">
+        <v>15</v>
+      </c>
+      <c r="X12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>15</v>
+      </c>
+      <c r="X13" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G14" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>35</v>
+      </c>
+      <c r="X14" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>30</v>
+      </c>
+      <c r="X15" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>112</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+      <c r="W16">
+        <v>35</v>
+      </c>
+      <c r="X16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>35</v>
+      </c>
+      <c r="X17" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" t="s">
+        <v>51</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>35</v>
+      </c>
+      <c r="X18" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" t="s">
+        <v>51</v>
+      </c>
+      <c r="K19" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="W19">
+        <v>30</v>
+      </c>
+      <c r="X19" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM19" t="s">
+        <v>129</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>1</v>
+      </c>
+      <c r="AP19" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ19" t="s">
+        <v>131</v>
+      </c>
+      <c r="AR19">
+        <v>1</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>30</v>
+      </c>
+      <c r="W20">
+        <v>35</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>138</v>
+      </c>
+      <c r="AO20">
+        <v>1</v>
+      </c>
+      <c r="AP20" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ20" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" t="s">
+        <v>52</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>35</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>125</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM21" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+      <c r="AP21" t="s">
+        <v>130</v>
+      </c>
+      <c r="AQ21" t="s">
+        <v>133</v>
+      </c>
+      <c r="AS21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+      <c r="K22" t="s">
+        <v>52</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>18</v>
+      </c>
+      <c r="X22" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>50</v>
+      </c>
+      <c r="G23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+      <c r="K23" t="s">
+        <v>52</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="W23">
+        <v>20</v>
+      </c>
+      <c r="X23" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>51</v>
+      </c>
+      <c r="K24" t="s">
+        <v>52</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="W24">
+        <v>20</v>
+      </c>
+      <c r="X24" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="W25">
+        <v>20</v>
+      </c>
+      <c r="X25" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL25" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM25" t="s">
+        <v>151</v>
+      </c>
+      <c r="AN25">
+        <v>0</v>
+      </c>
+      <c r="AO25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" t="s">
+        <v>52</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>20</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL26" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>155</v>
+      </c>
+      <c r="AO26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" t="s">
+        <v>157</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" t="s">
+        <v>52</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="W27">
+        <v>20</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>127</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>128</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>132</v>
+      </c>
+      <c r="AO27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" t="s">
+        <v>51</v>
+      </c>
+      <c r="K28" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="W28">
+        <v>20</v>
+      </c>
+      <c r="X28" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K29" t="s">
+        <v>52</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29">
+        <v>5</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="V29">
+        <v>18</v>
+      </c>
+      <c r="W29">
+        <v>20</v>
+      </c>
+      <c r="X29" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C0A549D-9CAE-4A9A-ABD4-E344B4A75FFB}">
+  <dimension ref="A1:AU29"/>
+  <sheetViews>
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>